<commit_message>
Deploy projeto Relatorio Vendas RPA
</commit_message>
<xml_diff>
--- a/Projetos-Github-RPA/Python/Open-AI-ChatGPT/Exemplo1.xlsx
+++ b/Projetos-Github-RPA/Python/Open-AI-ChatGPT/Exemplo1.xlsx
@@ -461,7 +461,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Ótimo trabalho, continue com excelência!</t>
+          <t>Great work, continue with excellence!</t>
         </is>
       </c>
     </row>
@@ -476,7 +476,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Meu nome é Daniel.</t>
+          <t>My name is Daniel.</t>
         </is>
       </c>
     </row>
@@ -491,7 +491,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Olá, esse é um teste utilizando a API da OpenAI para corrigir texto.</t>
+          <t>Hello, this is a test using the OpenAI API to correct text.</t>
         </is>
       </c>
     </row>
@@ -506,7 +506,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Eu acredito em você.</t>
+          <t>I believe in you.</t>
         </is>
       </c>
     </row>
@@ -521,7 +521,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Você tem um futuro brilhante pela frente. Siga em frente.</t>
+          <t>You have a bright future ahead. Keep moving forward.</t>
         </is>
       </c>
     </row>
@@ -536,7 +536,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Você é capaz de fazer coisas incríveis.</t>
+          <t>You are capable of doing incredible things.</t>
         </is>
       </c>
     </row>
@@ -551,7 +551,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Seu desempenho está melhorando a cada dia.</t>
+          <t>Your performance is improving every day.</t>
         </is>
       </c>
     </row>
@@ -566,7 +566,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Você é inteligente e estou orgulhoso disso.</t>
+          <t>You are intelligent and I am proud of it.</t>
         </is>
       </c>
     </row>
@@ -581,7 +581,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Seu esforço vale a pena.</t>
+          <t>Your effort is worth it.</t>
         </is>
       </c>
     </row>
@@ -596,7 +596,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Você é uma inspiração.</t>
+          <t>You are an inspiration.</t>
         </is>
       </c>
     </row>

</xml_diff>